<commit_message>
Make statu check more useful
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4CE445-32F9-45CC-A315-DCDAE309E210}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29864D5-ED09-42A5-B401-DD56F1F682DC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Password</t>
   </si>
@@ -78,7 +78,16 @@
     <t>DELETE</t>
   </si>
   <si>
-    <t>morga06</t>
+    <t>SubUrl</t>
+  </si>
+  <si>
+    <t>StatuCode</t>
+  </si>
+  <si>
+    <t>getMultipleServiceListing</t>
+  </si>
+  <si>
+    <t>ppp8989</t>
   </si>
 </sst>
 </file>
@@ -544,7 +553,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFFFBD6D-B83E-4C25-A3BA-2F64BB625EA6}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -552,7 +561,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -562,16 +571,28 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>